<commit_message>
M Newrifmutdata/Newmutdata/latestnewdata.xlsx  M Newrifmutdata/Newmutdata/newpaper.xlsx
</commit_message>
<xml_diff>
--- a/Newrifmutdata/Newmutdata/latestnewdata.xlsx
+++ b/Newrifmutdata/Newmutdata/latestnewdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="573">
   <si>
     <t>Species</t>
   </si>
@@ -1128,6 +1128,624 @@
   </si>
   <si>
     <t>Suppressor mutation allowing Δspx viability; selected in library screen under rif.</t>
+  </si>
+  <si>
+    <t>RM1</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>C1576G</t>
+  </si>
+  <si>
+    <t>CAC→GAC</t>
+  </si>
+  <si>
+    <t>H→D</t>
+  </si>
+  <si>
+    <t>H526D</t>
+  </si>
+  <si>
+    <t>RM+Rif100 µg/mL</t>
+  </si>
+  <si>
+    <t>Classic RRDR mutation H526D</t>
+  </si>
+  <si>
+    <t>Hayes2016</t>
+  </si>
+  <si>
+    <t>RM2</t>
+  </si>
+  <si>
+    <t>C1576T</t>
+  </si>
+  <si>
+    <t>Classic RRDR mutation H526Y</t>
+  </si>
+  <si>
+    <t>RM3</t>
+  </si>
+  <si>
+    <t>A&gt;G</t>
+  </si>
+  <si>
+    <t>A1577G</t>
+  </si>
+  <si>
+    <t>H526R</t>
+  </si>
+  <si>
+    <t>H526R new substitution</t>
+  </si>
+  <si>
+    <t>RM4</t>
+  </si>
+  <si>
+    <t>T1582C</t>
+  </si>
+  <si>
+    <t>TCG→CCG</t>
+  </si>
+  <si>
+    <t>S528</t>
+  </si>
+  <si>
+    <t>S528P</t>
+  </si>
+  <si>
+    <t>Non-hotspot mutation</t>
+  </si>
+  <si>
+    <t>RM5</t>
+  </si>
+  <si>
+    <t>C1585T</t>
+  </si>
+  <si>
+    <t>R529C novel substitution</t>
+  </si>
+  <si>
+    <t>RM6</t>
+  </si>
+  <si>
+    <t>C1592T</t>
+  </si>
+  <si>
+    <t>H531</t>
+  </si>
+  <si>
+    <t>H531Y</t>
+  </si>
+  <si>
+    <t>H531Y classic high-resistance mutation</t>
+  </si>
+  <si>
+    <t>RM7</t>
+  </si>
+  <si>
+    <t>C1592A</t>
+  </si>
+  <si>
+    <t>H531N</t>
+  </si>
+  <si>
+    <t>H531N high-resistance mutation</t>
+  </si>
+  <si>
+    <t>RM8</t>
+  </si>
+  <si>
+    <t>C1595A</t>
+  </si>
+  <si>
+    <t>A532</t>
+  </si>
+  <si>
+    <t>A532V</t>
+  </si>
+  <si>
+    <t>A532V substitution</t>
+  </si>
+  <si>
+    <t>RM9</t>
+  </si>
+  <si>
+    <t>G1600T</t>
+  </si>
+  <si>
+    <t>TGT</t>
+  </si>
+  <si>
+    <t>GGT→TGT</t>
+  </si>
+  <si>
+    <t>G534</t>
+  </si>
+  <si>
+    <t>G534C</t>
+  </si>
+  <si>
+    <t>G534C substitution</t>
+  </si>
+  <si>
+    <t>RM10</t>
+  </si>
+  <si>
+    <t>G1601A</t>
+  </si>
+  <si>
+    <t>GGC→GAC</t>
+  </si>
+  <si>
+    <t>G534D</t>
+  </si>
+  <si>
+    <t>G534D substitution</t>
+  </si>
+  <si>
+    <t>RM11</t>
+  </si>
+  <si>
+    <t>A1607G</t>
+  </si>
+  <si>
+    <t>ATC→GTC</t>
+  </si>
+  <si>
+    <t>I536</t>
+  </si>
+  <si>
+    <t>Ile</t>
+  </si>
+  <si>
+    <t>I→V</t>
+  </si>
+  <si>
+    <t>I536V</t>
+  </si>
+  <si>
+    <t>I536V substitution</t>
+  </si>
+  <si>
+    <t>RM12</t>
+  </si>
+  <si>
+    <t>A1547G</t>
+  </si>
+  <si>
+    <t>D516G classic RifR mutation</t>
+  </si>
+  <si>
+    <t>RM13</t>
+  </si>
+  <si>
+    <t>C1548T</t>
+  </si>
+  <si>
+    <t>GAC→GAT</t>
+  </si>
+  <si>
+    <t>D→D (silent)</t>
+  </si>
+  <si>
+    <t>D516D</t>
+  </si>
+  <si>
+    <t>Synonymous D516D mutation</t>
+  </si>
+  <si>
+    <t>RM14</t>
+  </si>
+  <si>
+    <t>A&gt;C</t>
+  </si>
+  <si>
+    <t>A1687C</t>
+  </si>
+  <si>
+    <t>ACC→GCC</t>
+  </si>
+  <si>
+    <t>T563</t>
+  </si>
+  <si>
+    <t>Thr</t>
+  </si>
+  <si>
+    <t>T→A</t>
+  </si>
+  <si>
+    <t>T563A</t>
+  </si>
+  <si>
+    <t>T563A substitution</t>
+  </si>
+  <si>
+    <t>RM15</t>
+  </si>
+  <si>
+    <t>T1590C</t>
+  </si>
+  <si>
+    <t>TAC→CAC</t>
+  </si>
+  <si>
+    <t>Y530</t>
+  </si>
+  <si>
+    <t>Y→H</t>
+  </si>
+  <si>
+    <t>Y530H</t>
+  </si>
+  <si>
+    <t>Y530H substitution</t>
+  </si>
+  <si>
+    <t>RM16</t>
+  </si>
+  <si>
+    <t>C1591A</t>
+  </si>
+  <si>
+    <t>H530</t>
+  </si>
+  <si>
+    <t>H530N</t>
+  </si>
+  <si>
+    <t>H530N mutation</t>
+  </si>
+  <si>
+    <t>RM17</t>
+  </si>
+  <si>
+    <t>C1691T</t>
+  </si>
+  <si>
+    <t>CCT</t>
+  </si>
+  <si>
+    <t>CCT→TCT</t>
+  </si>
+  <si>
+    <t>P564</t>
+  </si>
+  <si>
+    <t>P→S</t>
+  </si>
+  <si>
+    <t>P564S</t>
+  </si>
+  <si>
+    <t>P564S mutation</t>
+  </si>
+  <si>
+    <t>RM18</t>
+  </si>
+  <si>
+    <t>T&gt;G</t>
+  </si>
+  <si>
+    <t>T1573G</t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>ACT→GCT</t>
+  </si>
+  <si>
+    <t>T525</t>
+  </si>
+  <si>
+    <t>T525A</t>
+  </si>
+  <si>
+    <t>T525A mutation</t>
+  </si>
+  <si>
+    <t>RM19</t>
+  </si>
+  <si>
+    <t>G1549T</t>
+  </si>
+  <si>
+    <t>D517</t>
+  </si>
+  <si>
+    <t>D517D</t>
+  </si>
+  <si>
+    <t>Synonymous D517D mutation</t>
+  </si>
+  <si>
+    <t>RM20</t>
+  </si>
+  <si>
+    <t>A1587G</t>
+  </si>
+  <si>
+    <t>GCG</t>
+  </si>
+  <si>
+    <t>GGG</t>
+  </si>
+  <si>
+    <t>GCG→GGG</t>
+  </si>
+  <si>
+    <t>A529</t>
+  </si>
+  <si>
+    <t>A→G</t>
+  </si>
+  <si>
+    <t>A529G</t>
+  </si>
+  <si>
+    <t>A529G substitution</t>
+  </si>
+  <si>
+    <t>RM21</t>
+  </si>
+  <si>
+    <t>A1581T</t>
+  </si>
+  <si>
+    <t>GCT→GTT</t>
+  </si>
+  <si>
+    <t>A528</t>
+  </si>
+  <si>
+    <t>A528V</t>
+  </si>
+  <si>
+    <t>A528V substitution</t>
+  </si>
+  <si>
+    <t>RM22</t>
+  </si>
+  <si>
+    <t>T1546G</t>
+  </si>
+  <si>
+    <t>ACA</t>
+  </si>
+  <si>
+    <t>ACA→GCA</t>
+  </si>
+  <si>
+    <t>T515</t>
+  </si>
+  <si>
+    <t>T515A</t>
+  </si>
+  <si>
+    <t>T515A substitution</t>
+  </si>
+  <si>
+    <t>RM23</t>
+  </si>
+  <si>
+    <t>G1575T</t>
+  </si>
+  <si>
+    <t>A525</t>
+  </si>
+  <si>
+    <t>A525V</t>
+  </si>
+  <si>
+    <t>A525V substitution</t>
+  </si>
+  <si>
+    <t>RM24</t>
+  </si>
+  <si>
+    <t>H526N classic mutation</t>
+  </si>
+  <si>
+    <t>RM25</t>
+  </si>
+  <si>
+    <t>CAC→CAT</t>
+  </si>
+  <si>
+    <t>H→H (silent)</t>
+  </si>
+  <si>
+    <t>H526H</t>
+  </si>
+  <si>
+    <t>Synonymous H526H mutation</t>
+  </si>
+  <si>
+    <t>RM26</t>
+  </si>
+  <si>
+    <t>T1597C</t>
+  </si>
+  <si>
+    <t>T533</t>
+  </si>
+  <si>
+    <t>T533A</t>
+  </si>
+  <si>
+    <t>T533A substitution</t>
+  </si>
+  <si>
+    <t>RM27</t>
+  </si>
+  <si>
+    <t>A1583G</t>
+  </si>
+  <si>
+    <t>GCC→GGC</t>
+  </si>
+  <si>
+    <t>A528G</t>
+  </si>
+  <si>
+    <t>A528G substitution</t>
+  </si>
+  <si>
+    <t>RM28</t>
+  </si>
+  <si>
+    <t>C1688T</t>
+  </si>
+  <si>
+    <t>R563</t>
+  </si>
+  <si>
+    <t>R563C</t>
+  </si>
+  <si>
+    <t>R563C substitution</t>
+  </si>
+  <si>
+    <t>RM29</t>
+  </si>
+  <si>
+    <t>G1690A</t>
+  </si>
+  <si>
+    <t>G564</t>
+  </si>
+  <si>
+    <t>G564D</t>
+  </si>
+  <si>
+    <t>G564D substitution</t>
+  </si>
+  <si>
+    <t>RM30</t>
+  </si>
+  <si>
+    <t>A1689G</t>
+  </si>
+  <si>
+    <t>A564</t>
+  </si>
+  <si>
+    <t>A564G</t>
+  </si>
+  <si>
+    <t>A564G substitution</t>
+  </si>
+  <si>
+    <t>RM31</t>
+  </si>
+  <si>
+    <t>G1569A</t>
+  </si>
+  <si>
+    <t>G524</t>
+  </si>
+  <si>
+    <t>G524D</t>
+  </si>
+  <si>
+    <t>G524D substitution</t>
+  </si>
+  <si>
+    <t>RM32</t>
+  </si>
+  <si>
+    <t>D530</t>
+  </si>
+  <si>
+    <t>D530N mutation</t>
+  </si>
+  <si>
+    <t>RM33</t>
+  </si>
+  <si>
+    <t>G1686A</t>
+  </si>
+  <si>
+    <t>G562</t>
+  </si>
+  <si>
+    <t>G562D</t>
+  </si>
+  <si>
+    <t>G562D substitution</t>
+  </si>
+  <si>
+    <t>RM34</t>
+  </si>
+  <si>
+    <t>T1586C</t>
+  </si>
+  <si>
+    <t>G529D</t>
+  </si>
+  <si>
+    <t>G529D substitution</t>
+  </si>
+  <si>
+    <t>Enterococcus faecium</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>RifR mutant</t>
+  </si>
+  <si>
+    <t>G169A</t>
+  </si>
+  <si>
+    <t>G57</t>
+  </si>
+  <si>
+    <t>G57D</t>
+  </si>
+  <si>
+    <t>BHI+Rif20 µg/mL</t>
+  </si>
+  <si>
+    <t>Rifampin resistance mutation</t>
+  </si>
+  <si>
+    <t>Sacco2015</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>C473A</t>
+  </si>
+  <si>
+    <t>R158</t>
+  </si>
+  <si>
+    <t>R158H</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Rifampin resistance mutation (same as D2)</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>C473T</t>
+  </si>
+  <si>
+    <t>R158C</t>
+  </si>
+  <si>
+    <t>Rifampin resistance mutation (different amino acid)</t>
   </si>
 </sst>
 </file>
@@ -1751,7 +2369,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1766,6 +2384,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2292,10 +2916,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AB46"/>
+  <dimension ref="A1:AB88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:AB44"/>
+    <sheetView tabSelected="1" topLeftCell="I64" workbookViewId="0">
+      <selection activeCell="AB88" sqref="AB8:AB88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2982,9 +3606,7 @@
       <c r="AA8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AB8" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB8" s="2"/>
     </row>
     <row r="9" ht="72" spans="1:28">
       <c r="A9" s="2" t="s">
@@ -3068,9 +3690,7 @@
       <c r="AA9" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AB9" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB9" s="2"/>
     </row>
     <row r="10" ht="72" spans="1:28">
       <c r="A10" s="2" t="s">
@@ -3154,9 +3774,7 @@
       <c r="AA10" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AB10" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB10" s="2"/>
     </row>
     <row r="11" ht="57.6" spans="1:28">
       <c r="A11" s="2" t="s">
@@ -3240,9 +3858,7 @@
       <c r="AA11" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AB11" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB11" s="2"/>
     </row>
     <row r="12" ht="144" spans="1:28">
       <c r="A12" s="2" t="s">
@@ -3326,9 +3942,7 @@
       <c r="AA12" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AB12" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB12" s="2"/>
     </row>
     <row r="13" spans="1:28">
       <c r="A13" s="1"/>
@@ -3442,9 +4056,7 @@
       <c r="AA14" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AB14" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB14" s="2"/>
     </row>
     <row r="15" ht="115.2" spans="1:28">
       <c r="A15" s="2" t="s">
@@ -3528,9 +4140,7 @@
       <c r="AA15" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AB15" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB15" s="2"/>
     </row>
     <row r="16" ht="115.2" spans="1:28">
       <c r="A16" s="2" t="s">
@@ -3614,9 +4224,7 @@
       <c r="AA16" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AB16" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB16" s="2"/>
     </row>
     <row r="17" ht="72" spans="1:28">
       <c r="A17" s="2" t="s">
@@ -3700,9 +4308,7 @@
       <c r="AA17" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AB17" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB17" s="2"/>
     </row>
     <row r="18" spans="1:28">
       <c r="A18" s="1"/>
@@ -3816,9 +4422,7 @@
       <c r="AA19" t="s">
         <v>208</v>
       </c>
-      <c r="AB19" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB19" s="2"/>
     </row>
     <row r="20" ht="57.6" spans="1:28">
       <c r="A20" s="2" t="s">
@@ -3902,9 +4506,7 @@
       <c r="AA20" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AB20" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB20" s="2"/>
     </row>
     <row r="21" ht="72" spans="1:28">
       <c r="A21" s="2" t="s">
@@ -3988,9 +4590,7 @@
       <c r="AA21" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AB21" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB21" s="2"/>
     </row>
     <row r="22" ht="57.6" spans="1:28">
       <c r="A22" s="2" t="s">
@@ -4074,9 +4674,7 @@
       <c r="AA22" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AB22" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB22" s="2"/>
     </row>
     <row r="23" ht="57.6" spans="1:28">
       <c r="A23" s="2" t="s">
@@ -4160,9 +4758,7 @@
       <c r="AA23" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AB23" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB23" s="2"/>
     </row>
     <row r="24" ht="72" spans="1:28">
       <c r="A24" s="2" t="s">
@@ -4246,9 +4842,7 @@
       <c r="AA24" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AB24" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB24" s="2"/>
     </row>
     <row r="25" ht="100.8" spans="1:28">
       <c r="A25" s="2" t="s">
@@ -4332,9 +4926,7 @@
       <c r="AA25" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AB25" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB25" s="2"/>
     </row>
     <row r="26" ht="86.4" spans="1:28">
       <c r="A26" s="2" t="s">
@@ -4418,9 +5010,7 @@
       <c r="AA26" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AB26" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB26" s="2"/>
     </row>
     <row r="27" spans="1:28">
       <c r="A27" s="1"/>
@@ -4534,9 +5124,7 @@
       <c r="AA28" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="AB28" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB28" s="2"/>
     </row>
     <row r="29" ht="129.6" spans="1:28">
       <c r="A29" s="2" t="s">
@@ -4620,9 +5208,7 @@
       <c r="AA29" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="AB29" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB29" s="2"/>
     </row>
     <row r="30" ht="86.4" spans="1:28">
       <c r="A30" s="2" t="s">
@@ -4706,9 +5292,7 @@
       <c r="AA30" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="AB30" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB30" s="2"/>
     </row>
     <row r="31" spans="1:28">
       <c r="A31" s="1"/>
@@ -4822,9 +5406,7 @@
       <c r="AA32" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="AB32" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB32" s="2"/>
     </row>
     <row r="33" spans="1:28">
       <c r="A33" s="1"/>
@@ -4938,9 +5520,7 @@
       <c r="AA34" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="AB34" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB34" s="2"/>
     </row>
     <row r="35" ht="100.8" spans="1:28">
       <c r="A35" s="2" t="s">
@@ -5024,9 +5604,7 @@
       <c r="AA35" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="AB35" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB35" s="2"/>
     </row>
     <row r="36" ht="72" spans="1:28">
       <c r="A36" s="2" t="s">
@@ -5224,9 +5802,7 @@
       <c r="AA38" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="AB38" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB38" s="2"/>
     </row>
     <row r="39" spans="1:28">
       <c r="A39" s="3"/>
@@ -5340,9 +5916,7 @@
       <c r="AA40" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="AB40" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB40" s="4"/>
     </row>
     <row r="41" ht="187.2" spans="1:28">
       <c r="A41" s="4" t="s">
@@ -5426,9 +6000,7 @@
       <c r="AA41" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="AB41" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB41" s="4"/>
     </row>
     <row r="42" spans="1:28">
       <c r="A42" s="3"/>
@@ -5542,9 +6114,7 @@
       <c r="AA43" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="AB43" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB43" s="4"/>
     </row>
     <row r="44" spans="1:28">
       <c r="A44" s="3"/>
@@ -5658,9 +6228,7 @@
       <c r="AA45" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="AB45" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB45" s="4"/>
     </row>
     <row r="46" ht="187.2" spans="1:28">
       <c r="A46" s="4" t="s">
@@ -5744,9 +6312,3337 @@
       <c r="AA46" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="AB46" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB46" s="4"/>
+    </row>
+    <row r="47" ht="43.2" spans="1:28">
+      <c r="A47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P47" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q47" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R47" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S47" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T47" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U47" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="V47" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="W47" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="X47" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z47" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA47" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB47" s="5"/>
+    </row>
+    <row r="48" ht="57.6" spans="1:28">
+      <c r="A48" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" s="6">
+        <v>1576</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M48" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="O48" s="6">
+        <v>526</v>
+      </c>
+      <c r="P48" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R48" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="S48" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="T48" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="V48" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W48" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X48" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y48" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z48" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="AA48" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB48" s="6"/>
+    </row>
+    <row r="49" ht="57.6" spans="1:28">
+      <c r="A49" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" s="6">
+        <v>1576</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M49" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="N49" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="O49" s="6">
+        <v>526</v>
+      </c>
+      <c r="P49" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q49" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R49" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="S49" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="T49" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="V49" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W49" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X49" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y49" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z49" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="AA49" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB49" s="6"/>
+    </row>
+    <row r="50" ht="57.6" spans="1:28">
+      <c r="A50" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" s="6">
+        <v>1577</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M50" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N50" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O50" s="6">
+        <v>526</v>
+      </c>
+      <c r="P50" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q50" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R50" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="S50" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="T50" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="V50" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W50" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X50" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y50" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z50" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="AA50" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB50" s="6"/>
+    </row>
+    <row r="51" ht="43.2" spans="1:28">
+      <c r="A51" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" s="6">
+        <v>1582</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M51" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N51" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="O51" s="6">
+        <v>528</v>
+      </c>
+      <c r="P51" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q51" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="R51" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="S51" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="T51" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="V51" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W51" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X51" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y51" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z51" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="AA51" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB51" s="6"/>
+    </row>
+    <row r="52" ht="57.6" spans="1:28">
+      <c r="A52" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" s="6">
+        <v>1585</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="O52" s="6">
+        <v>529</v>
+      </c>
+      <c r="P52" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q52" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R52" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="S52" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="T52" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="V52" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W52" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X52" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y52" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z52" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="AA52" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB52" s="6"/>
+    </row>
+    <row r="53" ht="86.4" spans="1:28">
+      <c r="A53" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" s="6">
+        <v>1592</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M53" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="N53" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="O53" s="6">
+        <v>531</v>
+      </c>
+      <c r="P53" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q53" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R53" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="S53" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="T53" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="V53" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W53" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X53" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y53" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z53" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="AA53" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB53" s="6"/>
+    </row>
+    <row r="54" ht="72" spans="1:28">
+      <c r="A54" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="6">
+        <v>1592</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M54" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="N54" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="O54" s="6">
+        <v>531</v>
+      </c>
+      <c r="P54" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q54" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R54" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="S54" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="T54" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="V54" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W54" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X54" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y54" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z54" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA54" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB54" s="6"/>
+    </row>
+    <row r="55" ht="43.2" spans="1:28">
+      <c r="A55" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E55" s="6">
+        <v>1595</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="M55" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="O55" s="6">
+        <v>532</v>
+      </c>
+      <c r="P55" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="Q55" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="R55" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="S55" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="T55" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="V55" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W55" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X55" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y55" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z55" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="AA55" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB55" s="6"/>
+    </row>
+    <row r="56" ht="43.2" spans="1:28">
+      <c r="A56" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E56" s="6">
+        <v>1600</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="L56" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="M56" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="N56" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="O56" s="6">
+        <v>534</v>
+      </c>
+      <c r="P56" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q56" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="R56" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="S56" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="T56" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="V56" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W56" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X56" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y56" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z56" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="AA56" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB56" s="6"/>
+    </row>
+    <row r="57" ht="43.2" spans="1:28">
+      <c r="A57" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" s="6">
+        <v>1601</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="L57" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="M57" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N57" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="O57" s="6">
+        <v>534</v>
+      </c>
+      <c r="P57" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q57" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="R57" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="S57" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="T57" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="V57" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W57" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X57" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y57" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z57" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="AA57" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB57" s="6"/>
+    </row>
+    <row r="58" ht="28.8" spans="1:28">
+      <c r="A58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="5"/>
+      <c r="T58" s="5"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5"/>
+      <c r="Z58" s="5"/>
+      <c r="AA58" s="5"/>
+      <c r="AB58" s="5"/>
+    </row>
+    <row r="59" ht="43.2" spans="1:28">
+      <c r="A59" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" s="6">
+        <v>1607</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="L59" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="M59" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="N59" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="O59" s="6">
+        <v>536</v>
+      </c>
+      <c r="P59" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q59" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="R59" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="S59" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="T59" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="V59" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W59" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X59" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y59" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z59" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="AA59" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB59" s="6"/>
+    </row>
+    <row r="60" ht="57.6" spans="1:28">
+      <c r="A60" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E60" s="6">
+        <v>1547</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M60" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="N60" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="O60" s="6">
+        <v>516</v>
+      </c>
+      <c r="P60" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q60" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="R60" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="S60" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="T60" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="V60" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W60" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X60" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y60" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z60" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="AA60" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB60" s="6"/>
+    </row>
+    <row r="61" ht="43.2" spans="1:28">
+      <c r="A61" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" s="6">
+        <v>1548</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="L61" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M61" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="N61" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="O61" s="6">
+        <v>516</v>
+      </c>
+      <c r="P61" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q61" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="R61" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="S61" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="T61" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="V61" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W61" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X61" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y61" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z61" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="AA61" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB61" s="6"/>
+    </row>
+    <row r="62" ht="43.2" spans="1:28">
+      <c r="A62" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E62" s="6">
+        <v>1687</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="K62" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="L62" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="M62" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="N62" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="O62" s="6">
+        <v>563</v>
+      </c>
+      <c r="P62" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q62" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="R62" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="S62" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="T62" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="V62" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W62" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X62" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y62" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z62" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AA62" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB62" s="6"/>
+    </row>
+    <row r="63" ht="43.2" spans="1:28">
+      <c r="A63" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E63" s="6">
+        <v>1590</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J63" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="L63" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M63" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N63" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="O63" s="6">
+        <v>530</v>
+      </c>
+      <c r="P63" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="Q63" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="R63" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="S63" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="T63" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="V63" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W63" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X63" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y63" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z63" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AA63" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB63" s="6"/>
+    </row>
+    <row r="64" ht="28.8" spans="1:28">
+      <c r="A64" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E64" s="6">
+        <v>1591</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="L64" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M64" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="O64" s="6">
+        <v>530</v>
+      </c>
+      <c r="P64" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q64" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R64" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="S64" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="T64" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="V64" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W64" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X64" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y64" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z64" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="AA64" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB64" s="6"/>
+    </row>
+    <row r="65" ht="28.8" spans="1:28">
+      <c r="A65" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" s="6">
+        <v>1691</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="L65" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="M65" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="N65" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="O65" s="6">
+        <v>564</v>
+      </c>
+      <c r="P65" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q65" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R65" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S65" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="T65" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="V65" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W65" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X65" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y65" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z65" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="AA65" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB65" s="6"/>
+    </row>
+    <row r="66" ht="28.8" spans="1:28">
+      <c r="A66" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E66" s="6">
+        <v>1573</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="L66" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="M66" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="N66" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="O66" s="6">
+        <v>525</v>
+      </c>
+      <c r="P66" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="Q66" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="R66" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="S66" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="T66" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="V66" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W66" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X66" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y66" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z66" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AA66" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB66" s="6"/>
+    </row>
+    <row r="67" ht="43.2" spans="1:28">
+      <c r="A67" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" s="6">
+        <v>1549</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="L67" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M67" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="O67" s="6">
+        <v>517</v>
+      </c>
+      <c r="P67" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q67" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="R67" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="S67" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="T67" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="V67" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W67" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X67" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y67" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z67" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AA67" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB67" s="6"/>
+    </row>
+    <row r="68" ht="43.2" spans="1:28">
+      <c r="A68" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E68" s="6">
+        <v>1587</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="K68" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="L68" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="M68" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="O68" s="6">
+        <v>529</v>
+      </c>
+      <c r="P68" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q68" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="R68" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="S68" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="T68" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="V68" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W68" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X68" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y68" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z68" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="AA68" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB68" s="6"/>
+    </row>
+    <row r="69" spans="1:28">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
+      <c r="O69" s="5"/>
+      <c r="P69" s="5"/>
+      <c r="Q69" s="5"/>
+      <c r="R69" s="5"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="5"/>
+      <c r="V69" s="5"/>
+      <c r="W69" s="5"/>
+      <c r="X69" s="5"/>
+      <c r="Y69" s="5"/>
+      <c r="Z69" s="5"/>
+      <c r="AA69" s="5"/>
+      <c r="AB69" s="5"/>
+    </row>
+    <row r="70" ht="43.2" spans="1:28">
+      <c r="A70" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E70" s="6">
+        <v>1581</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="K70" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="L70" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="M70" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="N70" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="O70" s="6">
+        <v>528</v>
+      </c>
+      <c r="P70" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q70" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="R70" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="S70" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="T70" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="V70" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W70" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X70" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y70" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z70" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="AA70" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB70" s="6"/>
+    </row>
+    <row r="71" ht="43.2" spans="1:28">
+      <c r="A71" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E71" s="6">
+        <v>1546</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="L71" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="M71" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="N71" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="O71" s="6">
+        <v>515</v>
+      </c>
+      <c r="P71" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q71" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="R71" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="S71" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="T71" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="V71" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W71" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X71" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y71" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z71" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="AA71" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB71" s="6"/>
+    </row>
+    <row r="72" ht="43.2" spans="1:28">
+      <c r="A72" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E72" s="6">
+        <v>1575</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="L72" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="M72" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="N72" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="O72" s="6">
+        <v>525</v>
+      </c>
+      <c r="P72" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q72" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="R72" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="S72" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="T72" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="V72" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W72" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X72" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y72" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z72" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="AA72" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB72" s="6"/>
+    </row>
+    <row r="73" ht="43.2" spans="1:28">
+      <c r="A73" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E73" s="6">
+        <v>1576</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="L73" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M73" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="N73" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="O73" s="6">
+        <v>526</v>
+      </c>
+      <c r="P73" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q73" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R73" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="S73" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="T73" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="V73" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W73" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X73" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y73" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z73" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="AA73" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB73" s="6"/>
+    </row>
+    <row r="74" ht="43.2" spans="1:28">
+      <c r="A74" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E74" s="6">
+        <v>1578</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I74" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="L74" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M74" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="N74" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="O74" s="6">
+        <v>526</v>
+      </c>
+      <c r="P74" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q74" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R74" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="S74" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="T74" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="V74" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W74" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X74" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y74" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z74" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="AA74" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB74" s="6"/>
+    </row>
+    <row r="75" ht="43.2" spans="1:28">
+      <c r="A75" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E75" s="6">
+        <v>1597</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="L75" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="M75" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="N75" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="O75" s="6">
+        <v>533</v>
+      </c>
+      <c r="P75" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q75" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="R75" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="S75" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="T75" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="V75" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W75" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X75" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y75" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z75" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="AA75" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB75" s="6"/>
+    </row>
+    <row r="76" ht="43.2" spans="1:28">
+      <c r="A76" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E76" s="6">
+        <v>1583</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I76" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="L76" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="M76" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="N76" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="O76" s="6">
+        <v>528</v>
+      </c>
+      <c r="P76" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q76" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="R76" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="S76" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="T76" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="V76" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W76" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X76" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y76" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z76" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="AA76" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB76" s="6"/>
+    </row>
+    <row r="77" ht="43.2" spans="1:28">
+      <c r="A77" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E77" s="6">
+        <v>1688</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="L77" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M77" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N77" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="O77" s="6">
+        <v>563</v>
+      </c>
+      <c r="P77" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="Q77" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R77" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="S77" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="T77" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="V77" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W77" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X77" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y77" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z77" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="AA77" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB77" s="6"/>
+    </row>
+    <row r="78" ht="43.2" spans="1:28">
+      <c r="A78" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E78" s="6">
+        <v>1690</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H78" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I78" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="L78" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="M78" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N78" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="O78" s="6">
+        <v>564</v>
+      </c>
+      <c r="P78" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q78" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="R78" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="S78" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="T78" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="V78" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W78" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X78" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y78" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z78" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="AA78" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB78" s="6"/>
+    </row>
+    <row r="79" ht="43.2" spans="1:28">
+      <c r="A79" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" s="6">
+        <v>1689</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="K79" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="L79" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="M79" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="N79" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="O79" s="6">
+        <v>564</v>
+      </c>
+      <c r="P79" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q79" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="R79" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="S79" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="T79" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="V79" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W79" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X79" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y79" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z79" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="AA79" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB79" s="6"/>
+    </row>
+    <row r="80" ht="43.2" spans="1:28">
+      <c r="A80" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E80" s="6">
+        <v>1569</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I80" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J80" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="K80" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="L80" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="M80" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N80" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="O80" s="6">
+        <v>524</v>
+      </c>
+      <c r="P80" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q80" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="R80" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="S80" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="T80" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="V80" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W80" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X80" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y80" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z80" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="AA80" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB80" s="6"/>
+    </row>
+    <row r="81" ht="28.8" spans="1:28">
+      <c r="A81" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E81" s="6">
+        <v>1588</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="K81" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="L81" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M81" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="N81" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="O81" s="6">
+        <v>530</v>
+      </c>
+      <c r="P81" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q81" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="R81" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="S81" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="T81" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="V81" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W81" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X81" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y81" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z81" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="AA81" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB81" s="6"/>
+    </row>
+    <row r="82" ht="43.2" spans="1:28">
+      <c r="A82" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E82" s="6">
+        <v>1686</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J82" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="L82" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="M82" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="N82" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="O82" s="6">
+        <v>562</v>
+      </c>
+      <c r="P82" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="Q82" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="R82" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="S82" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="T82" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="V82" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W82" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X82" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y82" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z82" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="AA82" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB82" s="6"/>
+    </row>
+    <row r="83" ht="43.2" spans="1:28">
+      <c r="A83" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E83" s="6">
+        <v>1586</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H83" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I83" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J83" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="K83" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="L83" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="M83" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N83" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="O83" s="6">
+        <v>529</v>
+      </c>
+      <c r="P83" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q83" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="R83" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="S83" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="T83" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="V83" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="W83" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X83" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y83" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z83" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="AA83" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB83" s="6"/>
+    </row>
+    <row r="84" ht="43.2" spans="1:28">
+      <c r="A84" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K84" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L84" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M84" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N84" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O84" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P84" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q84" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R84" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S84" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T84" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U84" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="V84" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="W84" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="X84" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y84" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z84" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA84" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB84" s="5"/>
+    </row>
+    <row r="85" ht="57.6" spans="1:28">
+      <c r="A85" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I85" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="K85" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="L85" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="M85" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N85" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="O85" s="6">
+        <v>57</v>
+      </c>
+      <c r="P85" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="Q85" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="R85" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="S85" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="T85" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="U85" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="V85" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="W85" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X85" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y85" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z85" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="AA85" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="AB85" s="6"/>
+    </row>
+    <row r="86" ht="57.6" spans="1:28">
+      <c r="A86" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="K86" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="L86" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M86" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N86" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="O86" s="6">
+        <v>158</v>
+      </c>
+      <c r="P86" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="Q86" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R86" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="S86" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="T86" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="U86" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="V86" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="W86" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X86" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y86" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z86" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="AA86" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="AB86" s="6"/>
+    </row>
+    <row r="87" ht="86.4" spans="1:28">
+      <c r="A87" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="L87" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M87" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N87" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="O87" s="6">
+        <v>158</v>
+      </c>
+      <c r="P87" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="Q87" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R87" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="S87" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="T87" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="U87" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="V87" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="W87" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X87" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y87" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z87" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="AA87" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="AB87" s="6"/>
+    </row>
+    <row r="88" ht="100.8" spans="1:28">
+      <c r="A88" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="L88" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M88" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N88" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="O88" s="6">
+        <v>158</v>
+      </c>
+      <c r="P88" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="Q88" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R88" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="S88" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="T88" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="U88" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="V88" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="W88" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="X88" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y88" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z88" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="AA88" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="AB88" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>